<commit_message>
Manually Identified Domain Knowledge
</commit_message>
<xml_diff>
--- a/SampledOpenSourceProjects/SampledOpenSourceProjectsSummary.xlsx
+++ b/SampledOpenSourceProjects/SampledOpenSourceProjectsSummary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maggiema21/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maggiema21/SANER2018RENE/SampledOpenSourceProjects/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2306,10 +2306,10 @@
     <t>-AngularJsMasteringWebApp</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>URL</t>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Git URL</t>
   </si>
 </sst>
 </file>
@@ -2635,7 +2635,7 @@
   <dimension ref="A1:B381"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>